<commit_message>
Chart Project reading xlxs sheet with home, employees, project and chart page.
</commit_message>
<xml_diff>
--- a/data/22_07_20__Mitarbeiterplanung_InES_BH.xlsx
+++ b/data/22_07_20__Mitarbeiterplanung_InES_BH.xlsx
@@ -1796,13 +1796,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -1944,7 +1944,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1952,7 +1952,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1960,14 +1960,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1982,52 +1983,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2041,9 +1997,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2058,9 +2013,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2073,15 +2028,55 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -2093,6 +2088,11 @@
       <sz val="9"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -2182,79 +2182,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2272,7 +2200,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2284,25 +2260,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2320,13 +2320,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2338,13 +2338,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3168,15 +3168,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -3193,32 +3184,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3255,6 +3220,41 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -3264,142 +3264,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="72" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="72" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="69" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="69" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="68" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="70" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="71" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="68" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="67" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="66" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="67" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="66" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="71" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="65" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="65" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="66" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="66" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="27" borderId="70" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="67" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3417,7 +3417,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3425,18 +3425,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3489,7 +3489,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3499,7 +3499,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3524,7 +3524,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3533,41 +3533,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3577,14 +3577,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3599,10 +3599,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3611,16 +3611,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3636,11 +3636,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3652,7 +3652,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3685,10 +3685,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3705,61 +3705,61 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3774,96 +3774,96 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="5" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="5" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="7" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="7" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="6" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="11" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="11" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="8" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3873,24 +3873,24 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3921,7 +3921,7 @@
     <xf numFmtId="1" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3929,41 +3929,41 @@
     <xf numFmtId="1" fontId="2" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="10" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3974,64 +3974,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="9" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="17" fillId="10" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="17" fillId="10" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4039,30 +4039,30 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="17" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="17" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="17" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="17" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="3" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4109,35 +4109,35 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="12" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="2" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="12" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="2" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4465,10 +4465,10 @@
   <sheetPr/>
   <dimension ref="A1:CD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="104" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="12" topLeftCell="R1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="104" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="12" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A17" sqref="$A17:$XFD17"/>
+      <selection pane="topRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14"/>
@@ -4481,7 +4481,7 @@
     <col min="6" max="6" width="6" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="8" width="6.859375" customWidth="1"/>
-    <col min="9" max="9" width="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="1.4921875" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="4.7109375" customWidth="1"/>
     <col min="11" max="11" width="4.2890625" customWidth="1"/>
     <col min="12" max="14" width="4.7109375" customWidth="1"/>
@@ -4970,7 +4970,7 @@
       <c r="CC5" s="2"/>
       <c r="CD5" s="2"/>
     </row>
-    <row r="6" ht="14.75" spans="1:82">
+    <row r="6" spans="1:82">
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
@@ -5414,7 +5414,7 @@
       <c r="CC8" s="2"/>
       <c r="CD8" s="2"/>
     </row>
-    <row r="9" ht="14.75" spans="1:82">
+    <row r="9" ht="16" customHeight="1" spans="1:82">
       <c r="A9" s="307" t="s">
         <v>66</v>
       </c>
@@ -9135,10 +9135,10 @@
   <sheetPr/>
   <dimension ref="A1:BS37"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="8" topLeftCell="V1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" topLeftCell="A8" workbookViewId="0">
+      <pane xSplit="8" topLeftCell="AN1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A18" sqref="$A18:$XFD18"/>
+      <selection pane="topRight" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14"/>
@@ -9528,7 +9528,7 @@
       <c r="BQ7" s="43"/>
       <c r="BR7" s="44"/>
     </row>
-    <row r="8" spans="1:70">
+    <row r="8" ht="14.75" spans="1:70">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
         <v>64</v>
@@ -9666,7 +9666,7 @@
       <c r="BQ8" s="43"/>
       <c r="BR8" s="44"/>
     </row>
-    <row r="9" spans="1:70">
+    <row r="9" ht="14.75" spans="1:70">
       <c r="A9" s="11" t="s">
         <v>130</v>
       </c>
@@ -9776,7 +9776,7 @@
       <c r="BQ9" s="47"/>
       <c r="BR9" s="48"/>
     </row>
-    <row r="10" spans="1:70">
+    <row r="10" ht="14.75" spans="1:70">
       <c r="A10" s="14" t="s">
         <v>71</v>
       </c>
@@ -12591,10 +12591,10 @@
   <sheetPr/>
   <dimension ref="A1:BD37"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="J20" sqref="J20"/>
+      <selection pane="topRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14"/>
@@ -13007,7 +13007,7 @@
       <c r="BC8" s="2"/>
       <c r="BD8" s="2"/>
     </row>
-    <row r="9" ht="14.75" spans="1:56">
+    <row r="9" spans="1:56">
       <c r="A9" s="11" t="s">
         <v>140</v>
       </c>
@@ -13035,7 +13035,6 @@
       <c r="M9" s="9"/>
       <c r="N9" s="45"/>
       <c r="O9" s="101">
-        <f>'2023'!O32</f>
         <v>26</v>
       </c>
       <c r="P9" s="9"/>
@@ -13046,7 +13045,6 @@
       <c r="S9" s="102"/>
       <c r="T9" s="114"/>
       <c r="U9" s="128">
-        <f>12+'2023'!X32</f>
         <v>12</v>
       </c>
       <c r="V9" s="102"/>
@@ -15405,9 +15403,9 @@
   <dimension ref="A1:BN90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <pane xSplit="5" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="K11" sqref="K11"/>
+      <selection pane="topRight" activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14"/>
@@ -16018,7 +16016,7 @@
       <c r="BL8" s="44"/>
       <c r="BM8" s="2"/>
     </row>
-    <row r="9" ht="14.75" spans="1:65">
+    <row r="9" spans="1:65">
       <c r="A9" s="11" t="s">
         <v>156</v>
       </c>
@@ -16044,7 +16042,6 @@
       <c r="M9" s="9"/>
       <c r="N9" s="45"/>
       <c r="O9" s="101">
-        <f>'2024'!O32</f>
         <v>20</v>
       </c>
       <c r="P9" s="102"/>
@@ -16055,7 +16052,6 @@
       <c r="S9" s="9"/>
       <c r="T9" s="45"/>
       <c r="U9" s="127">
-        <f>'2024'!U32+5</f>
         <v>5</v>
       </c>
       <c r="V9" s="9"/>

</xml_diff>